<commit_message>
Update Mejzlik Static thrust calculator_Version1.xlsx
</commit_message>
<xml_diff>
--- a/Docs/Mejzlik Static thrust calculator_Version1.xlsx
+++ b/Docs/Mejzlik Static thrust calculator_Version1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\houte\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\houte\Desktop\Overig\Projects\Drone\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D270AFEB-B6E6-4DEA-AE52-46EA0B520A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E867A63-0559-4BBF-B949-3EFEF5B45C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="5CwDfsSqJ3zJAINzI9/E+IHCJUFNJMQc+NmDMm2S5qoXKN4ljZ8+BuhfFBN9+cI3GRLtS4hdoL70caZLVnUTOg==" workbookSaltValue="IcAj4za6fZe/NmMhGhgoew==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="848" firstSheet="1" activeTab="2" xr2:uid="{780D9684-9D4C-46B8-A3E3-2452F22A1FCD}"/>
@@ -3277,7 +3277,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>8262.273469514168</c:v>
+                  <c:v>3856.4608926298397</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3289,7 +3289,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.177925</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3991,7 +3991,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.177925</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4003,7 +4003,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>145.47861889712055</c:v>
+                  <c:v>11.434009174581668</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4678,7 +4678,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.177925</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4690,7 +4690,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6.8738623419787839</c:v>
+                  <c:v>15.561033517056776</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5769,7 +5769,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.177925</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5781,7 +5781,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5.4990898735830269</c:v>
+                  <c:v>12.44882681364542</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6205,31 +6205,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>181.84827362140064</c:v>
+                  <c:v>14.29251146822709</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>171.15131634955358</c:v>
+                  <c:v>13.451775499507852</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>161.64290988568945</c:v>
+                  <c:v>12.704454638424075</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>153.13538831275849</c:v>
+                  <c:v>12.035799131138598</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>145.47861889712055</c:v>
+                  <c:v>11.434009174581668</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>138.55106561630521</c:v>
+                  <c:v>10.889532547220643</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>132.25328990647327</c:v>
+                  <c:v>10.394553795074252</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>126.50314686706122</c:v>
+                  <c:v>9.9426166735492796</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>121.23218241426709</c:v>
+                  <c:v>9.5283409788180595</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6293,7 +6293,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>145.47861889712055</c:v>
+                  <c:v>11.434009174581668</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -6671,31 +6671,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>181.84827362140064</c:v>
+                  <c:v>14.29251146822709</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>171.15131634955358</c:v>
+                  <c:v>13.451775499507852</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>161.64290988568945</c:v>
+                  <c:v>12.704454638424075</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>153.13538831275849</c:v>
+                  <c:v>12.035799131138598</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>145.47861889712055</c:v>
+                  <c:v>11.434009174581668</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>138.55106561630521</c:v>
+                  <c:v>10.889532547220643</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>132.25328990647327</c:v>
+                  <c:v>10.394553795074252</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>126.50314686706122</c:v>
+                  <c:v>9.9426166735492796</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>121.23218241426709</c:v>
+                  <c:v>9.5283409788180595</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6738,7 +6738,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>145.47861889712055</c:v>
+                  <c:v>11.434009174581668</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -34868,7 +34868,7 @@
       </c>
       <c r="J6" s="30">
         <f ca="1">Calculator!G26</f>
-        <v>181.84827362140069</v>
+        <v>14.292511468227085</v>
       </c>
       <c r="L6" s="2">
         <v>0.44232081911262799</v>
@@ -34881,7 +34881,7 @@
       </c>
       <c r="P6" s="2">
         <f ca="1">J6/E6</f>
-        <v>0.86594416010190811</v>
+        <v>6.8059578420128969E-2</v>
       </c>
     </row>
     <row r="7" spans="4:16" ht="30.5" x14ac:dyDescent="0.6">
@@ -34898,7 +34898,7 @@
       </c>
       <c r="J7" s="30">
         <f ca="1">Calculator!G22</f>
-        <v>8262.273469514168</v>
+        <v>3856.4608926298397</v>
       </c>
       <c r="L7" s="2">
         <v>0.51331058020477816</v>
@@ -34911,7 +34911,7 @@
       </c>
       <c r="P7" s="2">
         <f ca="1">IFERROR(FORECAST(P6,OFFSET(M4:M11,MATCH(P6,L4:L11,1)-1,0,2),OFFSET(L4:L11,MATCH(P6,L4:L11,1)-1,0,2)),1)</f>
-        <v>0.80064895417217086</v>
+        <v>0.98188023382907597</v>
       </c>
     </row>
     <row r="8" spans="4:16" ht="30.5" x14ac:dyDescent="0.6">
@@ -34930,7 +34930,7 @@
       </c>
       <c r="J8" s="30">
         <f ca="1">J7/(0.76*E8)</f>
-        <v>979.40652791775346</v>
+        <v>457.14330163938354</v>
       </c>
       <c r="L8" s="2">
         <v>0.58134243458475543</v>
@@ -34945,7 +34945,7 @@
       </c>
       <c r="E9" s="29">
         <f ca="1">E8*E7*P7</f>
-        <v>12442.084747835535</v>
+        <v>15258.418833703841</v>
       </c>
       <c r="L9" s="2">
         <v>0.69055745164960181</v>
@@ -34974,15 +34974,15 @@
       </c>
       <c r="E11" s="31">
         <f ca="1">J7/(P7*E8)</f>
-        <v>929.68205021526626</v>
+        <v>353.84041482437192</v>
       </c>
       <c r="F11" s="31">
         <f>Calculator!E24</f>
-        <v>1</v>
+        <v>0.177925</v>
       </c>
       <c r="G11" s="30">
         <f ca="1">J6</f>
-        <v>181.84827362140069</v>
+        <v>14.292511468227085</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>98</v>
@@ -35104,15 +35104,15 @@
     <row r="19" spans="5:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E19" s="2">
         <f ca="1">_xlfn.FORECAST.LINEAR(E7,F11:F12,E11:E12)</f>
-        <v>1.5503769257476121</v>
+        <v>1.6328961470968038</v>
       </c>
       <c r="F19" s="2">
         <f ca="1">_xlfn.FORECAST.LINEAR(E7,G11:G12,E11:E12)</f>
-        <v>319.5283890701956</v>
+        <v>318.96316844456499</v>
       </c>
       <c r="G19" s="2">
         <f ca="1">E6-F19</f>
-        <v>-109.5283890701956</v>
+        <v>-108.96316844456499</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>134</v>
@@ -35488,8 +35488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5207784-2504-4C29-B22C-73D0D3988475}">
   <dimension ref="D13:Y69"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A38" zoomScale="49" zoomScaleNormal="30" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="34" zoomScaleNormal="34" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -35615,11 +35615,11 @@
       </c>
       <c r="G22" s="11">
         <f ca="1">Sheet1!AE3</f>
-        <v>8262.273469514168</v>
+        <v>3856.4608926298397</v>
       </c>
       <c r="H22" s="42">
         <f ca="1">G24/(G22*2*PI()/60)</f>
-        <v>0.16813997791593466</v>
+        <v>2.8312680410745063E-2</v>
       </c>
       <c r="J22" s="38"/>
       <c r="W22" s="39"/>
@@ -35645,15 +35645,15 @@
         <v>5</v>
       </c>
       <c r="E24" s="4">
-        <v>1</v>
+        <v>0.177925</v>
       </c>
       <c r="G24" s="9">
         <f ca="1">Sheet1!AE4</f>
-        <v>145.47861889712055</v>
+        <v>11.434009174581668</v>
       </c>
       <c r="H24" s="42">
         <f ca="1">+PI()*(E22*0.0254)*G22/60*0.00291545</f>
-        <v>0.32035942242605508</v>
+        <v>0.1495294955716602</v>
       </c>
       <c r="J24" s="38"/>
       <c r="W24" s="39"/>
@@ -35683,7 +35683,7 @@
       </c>
       <c r="G26" s="9">
         <f ca="1">G24/(E26/100)</f>
-        <v>181.84827362140069</v>
+        <v>14.292511468227085</v>
       </c>
       <c r="H26" s="45">
         <f>E22*0.33333</f>
@@ -35713,11 +35713,11 @@
       <c r="D28" s="38"/>
       <c r="G28" s="9">
         <f ca="1">E24*1000/G24</f>
-        <v>6.8738623419787839</v>
+        <v>15.561033517056776</v>
       </c>
       <c r="H28" s="42">
         <f ca="1">E24*1000/G26</f>
-        <v>5.4990898735830269</v>
+        <v>12.44882681364542</v>
       </c>
       <c r="I28" s="13"/>
       <c r="J28" s="38"/>
@@ -35747,7 +35747,7 @@
       </c>
       <c r="H30" s="42">
         <f ca="1">Sheet1!AE5</f>
-        <v>0.5312361038196447</v>
+        <v>0.50727525477802926</v>
       </c>
       <c r="J30" s="38"/>
       <c r="W30" s="39"/>
@@ -35871,7 +35871,7 @@
       </c>
       <c r="H41" s="36">
         <f ca="1">IF('Motor performance'!$F$13="Insufficient","",'Motor performance'!E11)</f>
-        <v>929.68205021526626</v>
+        <v>353.84041482437192</v>
       </c>
       <c r="J41" s="38"/>
       <c r="W41" s="39"/>
@@ -36005,7 +36005,7 @@
       </c>
       <c r="H52" s="42">
         <f ca="1">(E52*E53/1000*E54/100)/(G26*E55)*60</f>
-        <v>3.955385364270799</v>
+        <v>50.325654913693285</v>
       </c>
       <c r="I52" s="14"/>
     </row>
@@ -36022,7 +36022,7 @@
       </c>
       <c r="H53" s="42">
         <f ca="1">G26/E52</f>
-        <v>16.382727353279343</v>
+        <v>1.2876136457862239</v>
       </c>
     </row>
     <row r="54" spans="4:9" ht="30.5" x14ac:dyDescent="0.6">
@@ -36038,7 +36038,7 @@
       </c>
       <c r="H54" s="42">
         <f>E55*E24</f>
-        <v>4</v>
+        <v>0.7117</v>
       </c>
     </row>
     <row r="55" spans="4:9" ht="30.5" x14ac:dyDescent="0.6">
@@ -38597,7 +38597,7 @@
       </c>
       <c r="AE3" s="2">
         <f ca="1">IF(B6&lt;=W6,W9,IF(B6&gt;=Z6,Z9,W12))</f>
-        <v>8262.273469514168</v>
+        <v>3856.4608926298397</v>
       </c>
       <c r="AG3" s="2">
         <v>15</v>
@@ -38664,7 +38664,7 @@
       </c>
       <c r="AE4" s="2">
         <f ca="1">IF(B6&lt;=W6,X9,IF(B6&gt;=Z6,AA9,X12))</f>
-        <v>145.47861889712055</v>
+        <v>11.434009174581668</v>
       </c>
       <c r="AG4" s="2">
         <v>16</v>
@@ -38717,7 +38717,7 @@
       </c>
       <c r="AE5" s="2">
         <f ca="1">(((B6*9.81)/(B4*(200/60)^2*($B$1*0.0254)^4))^(3/2))/((AE4/(B4*((200/60)^3)*($B$1*0.0254)^5))*SQRT(2))</f>
-        <v>0.5312361038196447</v>
+        <v>0.50727525477802926</v>
       </c>
       <c r="AG5" s="2">
         <v>17</v>
@@ -38780,7 +38780,7 @@
       </c>
       <c r="B6" s="2">
         <f>Calculator!E24</f>
-        <v>1</v>
+        <v>0.177925</v>
       </c>
       <c r="L6" s="2">
         <f t="shared" ref="L6:L7" si="3">M5</f>
@@ -38829,7 +38829,7 @@
       </c>
       <c r="AP6" s="2">
         <f t="shared" ref="AP6:AP14" ca="1" si="4">(((($B$6*9.81)/($B$4*($AE$3/60)^2*($AO6*0.0254)^4))^(3/2))/($Y$12*SQRT(2))*($B$4*(($AE$3/60)^3)*($AO6*0.0254)^5))</f>
-        <v>181.84827362140064</v>
+        <v>14.29251146822709</v>
       </c>
       <c r="AQ6" s="2">
         <v>0</v>
@@ -38921,7 +38921,7 @@
       </c>
       <c r="AP7" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>171.15131634955358</v>
+        <v>13.451775499507852</v>
       </c>
       <c r="AQ7" s="2">
         <v>0</v>
@@ -38996,7 +38996,7 @@
       </c>
       <c r="AP8" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>161.64290988568945</v>
+        <v>12.704454638424075</v>
       </c>
       <c r="AQ8" s="2">
         <v>0</v>
@@ -39039,19 +39039,19 @@
       </c>
       <c r="W9" s="71">
         <f ca="1">SQRT(($B$6*9.81)/($B$4*($B$1*0.0254)^4*W4))*60</f>
-        <v>9244.6080689407154</v>
+        <v>3899.4826371745148</v>
       </c>
       <c r="X9" s="71">
         <f ca="1">X4*($B$4*((W9/60)^3)*($B$1*0.0254)^5)</f>
-        <v>148.20302895056128</v>
+        <v>11.122759363293389</v>
       </c>
       <c r="Z9" s="71">
         <f ca="1">SQRT(($B$6*9.81)/($B$4*($B$1*0.0254)^4*Z4))*60</f>
-        <v>8048.4383080888383</v>
+        <v>3394.9243931937553</v>
       </c>
       <c r="AA9" s="71">
         <f ca="1">AA4*($B$4*((Z9/60)^3)*($B$1*0.0254)^5)</f>
-        <v>140.28771566472076</v>
+        <v>10.528708583178414</v>
       </c>
       <c r="AG9" s="2">
         <v>24</v>
@@ -39065,7 +39065,7 @@
       </c>
       <c r="AP9" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>153.13538831275849</v>
+        <v>12.035799131138598</v>
       </c>
       <c r="AQ9" s="2">
         <v>0</v>
@@ -39125,11 +39125,11 @@
       </c>
       <c r="AP10" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>145.47861889712055</v>
+        <v>11.434009174581668</v>
       </c>
       <c r="AQ10" s="2">
         <f ca="1">AP10</f>
-        <v>145.47861889712055</v>
+        <v>11.434009174581668</v>
       </c>
       <c r="AV10" s="2" t="s">
         <v>18</v>
@@ -39199,7 +39199,7 @@
       </c>
       <c r="AP11" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>138.55106561630521</v>
+        <v>10.889532547220643</v>
       </c>
       <c r="AQ11" s="2">
         <v>0</v>
@@ -39256,15 +39256,15 @@
       </c>
       <c r="W12" s="2">
         <f ca="1">FORECAST($B6,OFFSET($A$51:$A$228,MATCH($B$6,$O$51:$O$228,1)-1,0,2),OFFSET($O$51:$O$228,MATCH($B$6,$O$51:$O$228,1)-1,0,2))</f>
-        <v>8262.273469514168</v>
+        <v>3856.4608926298397</v>
       </c>
       <c r="X12" s="2">
         <f ca="1">FORECAST($B6,OFFSET($P$51:$P$228,MATCH($B$6,$O$51:$O$228,1)-1,0,2),OFFSET($O$51:$O$228,MATCH($B$6,$O$51:$O$228,1)-1,0,2))</f>
-        <v>145.47861889712055</v>
+        <v>11.434009174581668</v>
       </c>
       <c r="Y12" s="2">
         <f ca="1">(((B6*9.81)/($B$4*($AE$3/60)^2*($B$1*0.0254)^4))^(3/2))/(($AE$4/($B$4*(($AE$3/60)^3)*($B$1*0.0254)^5))*SQRT(2))</f>
-        <v>0.53123610381964448</v>
+        <v>0.50727525477802948</v>
       </c>
       <c r="AG12" s="2">
         <v>30</v>
@@ -39278,7 +39278,7 @@
       </c>
       <c r="AP12" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>132.25328990647327</v>
+        <v>10.394553795074252</v>
       </c>
       <c r="AQ12" s="2">
         <v>0</v>
@@ -39331,7 +39331,7 @@
       </c>
       <c r="AP13" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>126.50314686706122</v>
+        <v>9.9426166735492796</v>
       </c>
       <c r="AQ13" s="2">
         <v>0</v>
@@ -39368,7 +39368,7 @@
       </c>
       <c r="AP14" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>121.23218241426709</v>
+        <v>9.5283409788180595</v>
       </c>
       <c r="AQ14" s="2">
         <v>0</v>
@@ -54263,15 +54263,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100024378DD67EC344A916D46CA3EAD196B" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5d8c3809a37c2cad34fe8b79b5722c05">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="53e77888-5bec-407a-a6fa-c2c7ee1e5467" xmlns:ns3="4548bcc8-bbdd-4d33-87dd-a61176a6844c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e14384a90a12b128e95202f65209c81b" ns2:_="" ns3:_="">
     <xsd:import namespace="53e77888-5bec-407a-a6fa-c2c7ee1e5467"/>
@@ -54482,6 +54473,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E0CE5D0-9C85-43E1-9AED-540A822003D7}">
   <ds:schemaRefs>
@@ -54500,14 +54500,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{902C0ABC-E1D1-4302-93BF-FB2A2A171540}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{774CB936-FDD5-434F-85F8-0AF4DFC0812B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -54524,4 +54516,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{902C0ABC-E1D1-4302-93BF-FB2A2A171540}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>